<commit_message>
Change sprites, fix controls, add win/lose and ui
</commit_message>
<xml_diff>
--- a/Docs/P.E.R Sheet.xlsx
+++ b/Docs/P.E.R Sheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C950C2-A33E-4ABA-A7EC-3278C467E128}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Setup Project</t>
+  </si>
+  <si>
+    <t>Setup Scene manager</t>
+  </si>
+  <si>
+    <t>Player Controls</t>
+  </si>
+  <si>
+    <t>Tree Collisions</t>
+  </si>
+  <si>
+    <t>Soldier Logic</t>
+  </si>
+  <si>
+    <t>Hospital Logic</t>
+  </si>
+  <si>
+    <t>Game Over/Win Screen</t>
+  </si>
+  <si>
+    <t>Assets/sprites</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +369,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>9.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>7.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>10.24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>26.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>